<commit_message>
changes of header names in data file
</commit_message>
<xml_diff>
--- a/Assignment 1/data.xlsx
+++ b/Assignment 1/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frede\Documents\DTU\2024\Renewables in Electricity Markets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frede\Documents\DTU\2024\Renewables in Electricity Markets\renew-in-elec-markets\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E93AA0-F396-46CC-9923-69B26E29E9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2698C1CF-FEB5-4489-BD4E-88ACC8F42682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gen_technical" sheetId="1" r:id="rId1"/>
@@ -109,10 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="117">
-  <si>
-    <t>Unit#</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="131">
   <si>
     <t>Node</t>
   </si>
@@ -124,9 +121,6 @@
   </si>
   <si>
     <t>R_{i}^{+}</t>
-  </si>
-  <si>
-    <t>R_{i}^{−}</t>
   </si>
   <si>
     <t>R_{i}^{U}</t>
@@ -399,12 +393,6 @@
 (MVA)</t>
   </si>
   <si>
-    <t>Load#</t>
-  </si>
-  <si>
-    <t>%ofsystemload</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -463,6 +451,60 @@
   </si>
   <si>
     <t>Numberofhoursofwhichthegeneratingunit i wasin/outatthebeginningofschedulinghorizon.</t>
+  </si>
+  <si>
+    <t>P_max</t>
+  </si>
+  <si>
+    <t>P_min</t>
+  </si>
+  <si>
+    <t>R_plus</t>
+  </si>
+  <si>
+    <t>R_minus</t>
+  </si>
+  <si>
+    <t>R_U</t>
+  </si>
+  <si>
+    <t>R_D</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C_u</t>
+  </si>
+  <si>
+    <t>C_d</t>
+  </si>
+  <si>
+    <t>C_plus</t>
+  </si>
+  <si>
+    <t>C_minus</t>
+  </si>
+  <si>
+    <t>C_su</t>
+  </si>
+  <si>
+    <t>P_ini</t>
+  </si>
+  <si>
+    <t>U_ini</t>
+  </si>
+  <si>
+    <t>T_ini</t>
+  </si>
+  <si>
+    <t>load_percent</t>
+  </si>
+  <si>
+    <t>Load</t>
   </si>
 </sst>
 </file>
@@ -506,7 +548,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,74 +831,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>113</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>114</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -867,28 +909,28 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -899,28 +941,28 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -931,28 +973,28 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -963,28 +1005,28 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="H6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -995,28 +1037,28 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1027,28 +1069,28 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1059,28 +1101,28 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1091,28 +1133,28 @@
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="H10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1123,28 +1165,28 @@
         <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="H11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1155,28 +1197,28 @@
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1187,28 +1229,28 @@
         <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1219,28 +1261,28 @@
         <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1253,73 +1295,73 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>120</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>121</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1327,31 +1369,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1359,31 +1401,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1391,31 +1433,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1423,31 +1465,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1455,31 +1497,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1487,31 +1529,31 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1519,31 +1561,31 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1551,31 +1593,31 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="J10" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1583,31 +1625,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1615,31 +1657,31 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="J12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1647,31 +1689,31 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1679,31 +1721,31 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1716,17 +1758,17 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1940,16 +1982,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2442,20 +2484,20 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2659,154 +2701,154 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDB7F6A-CE82-4E52-B255-E07EA147DBBD}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wind turbine introduction in bus network
</commit_message>
<xml_diff>
--- a/Assignment 1/data.xlsx
+++ b/Assignment 1/data.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frede\Documents\DTU\2024\Renewables in Electricity Markets\renew-in-elec-markets\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2698C1CF-FEB5-4489-BD4E-88ACC8F42682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC391156-33BA-418F-9434-728A03CAC72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gen_technical" sheetId="1" r:id="rId1"/>
     <sheet name="gen_cost" sheetId="2" r:id="rId2"/>
-    <sheet name="demand" sheetId="3" r:id="rId3"/>
-    <sheet name="transmission_line" sheetId="4" r:id="rId4"/>
-    <sheet name="demand_nodes" sheetId="5" r:id="rId5"/>
-    <sheet name="Nomenclature" sheetId="6" r:id="rId6"/>
+    <sheet name="wind_technical" sheetId="7" r:id="rId3"/>
+    <sheet name="demand" sheetId="3" r:id="rId4"/>
+    <sheet name="transmission_lines" sheetId="4" r:id="rId5"/>
+    <sheet name="demand_nodes" sheetId="5" r:id="rId6"/>
+    <sheet name="Nomenclature" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -109,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="127">
   <si>
     <t>Node</t>
   </si>
@@ -135,18 +136,6 @@
     <t>DT</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>(MW)</t>
-  </si>
-  <si>
-    <t>(MW/h)</t>
-  </si>
-  <si>
-    <t>(h)</t>
-  </si>
-  <si>
     <t>152</t>
   </si>
   <si>
@@ -261,15 +250,6 @@
     <t>T_{i}^{ini}</t>
   </si>
   <si>
-    <t>($/MWh)</t>
-  </si>
-  <si>
-    <t>($)</t>
-  </si>
-  <si>
-    <t>(0/1)</t>
-  </si>
-  <si>
     <t>13.32</t>
   </si>
   <si>
@@ -375,24 +355,12 @@
     <t>Hour</t>
   </si>
   <si>
-    <t>Systemdemand_x000D_
-(MW)</t>
-  </si>
-  <si>
     <t>From</t>
   </si>
   <si>
     <t>To</t>
   </si>
   <si>
-    <t>Reactance_x000D_
-(p.u.)</t>
-  </si>
-  <si>
-    <t>Capacity_x000D_
-(MVA)</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -505,6 +473,24 @@
   </si>
   <si>
     <t>Load</t>
+  </si>
+  <si>
+    <t>P_cap</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Capacity_wind</t>
+  </si>
+  <si>
+    <t>Reactance</t>
+  </si>
+  <si>
+    <t>System_demand</t>
+  </si>
+  <si>
+    <t>Profile</t>
   </si>
 </sst>
 </file>
@@ -546,9 +532,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,38 +818,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -870,145 +859,145 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="J4" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>23</v>
@@ -1017,30 +1006,30 @@
         <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>27</v>
@@ -1049,240 +1038,208 @@
         <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="J10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
         <v>12</v>
-      </c>
-      <c r="B14" s="1">
-        <v>23</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1292,125 +1249,125 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3A68B1-57DE-45FB-9142-3534A5100D62}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="1">
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>56</v>
@@ -1419,333 +1376,301 @@
         <v>57</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1754,21 +1679,248 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B09048F1-9A84-4E54-9031-5742F49396F2}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>200</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>200</v>
+      </c>
+      <c r="D3" s="1">
+        <v>94</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>200</v>
+      </c>
+      <c r="D4" s="1">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1">
+        <v>200</v>
+      </c>
+      <c r="D5" s="1">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1">
+        <v>200</v>
+      </c>
+      <c r="D6" s="1">
+        <v>46</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1">
+        <v>200</v>
+      </c>
+      <c r="D7" s="1">
+        <v>35</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3485FD-1017-4176-8D64-1DAAE0B61E3A}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1794,7 +1946,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>15.903</v>
+        <v>1590.3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1818,7 +1970,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>15.903</v>
+        <v>1590.3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1826,7 +1978,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>196.137</v>
+        <v>1961.37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1834,7 +1986,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>227.94300000000001</v>
+        <v>2279.4299999999998</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1850,7 +2002,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>254.44800000000001</v>
+        <v>2544.48</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1858,7 +2010,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>254.44800000000001</v>
+        <v>2544.48</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1914,7 +2066,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>26.504999999999999</v>
+        <v>2650.5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1922,7 +2074,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>26.504999999999999</v>
+        <v>2650.5</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1930,7 +2082,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>254.44800000000001</v>
+        <v>2544.48</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1963,515 +2115,6 @@
       </c>
       <c r="B25" s="1">
         <v>1669.8150000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D667A1-F40E-42FE-98A4-7969DB61290E}">
-  <dimension ref="A1:H35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.46E-2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.2253</v>
-      </c>
-      <c r="D3" s="1">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>9.0700000000000003E-2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.1356</v>
-      </c>
-      <c r="D5" s="1">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2.0500000000000001E-2</v>
-      </c>
-      <c r="D6" s="1">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.12710000000000002</v>
-      </c>
-      <c r="D7" s="1">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>24</v>
-      </c>
-      <c r="C8" s="1">
-        <v>8.4000000000000012E-3</v>
-      </c>
-      <c r="D8" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1.11E-2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1">
-        <v>9.4000000000000004E-3</v>
-      </c>
-      <c r="D10" s="1">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6.4200000000000007E-2</v>
-      </c>
-      <c r="D11" s="1">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1">
-        <v>6.5200000000000008E-2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0.1762</v>
-      </c>
-      <c r="D13" s="1">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>8</v>
-      </c>
-      <c r="B14" s="1">
-        <v>10</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0.1762</v>
-      </c>
-      <c r="D14" s="1">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1">
-        <v>11</v>
-      </c>
-      <c r="C15" s="1">
-        <v>8.4000000000000012E-3</v>
-      </c>
-      <c r="D15" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1">
-        <v>12</v>
-      </c>
-      <c r="C16" s="1">
-        <v>8.4000000000000012E-3</v>
-      </c>
-      <c r="D16" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>10</v>
-      </c>
-      <c r="B17" s="1">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1">
-        <v>8.4000000000000012E-3</v>
-      </c>
-      <c r="D17" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>10</v>
-      </c>
-      <c r="B18" s="1">
-        <v>12</v>
-      </c>
-      <c r="C18" s="1">
-        <v>8.4000000000000012E-3</v>
-      </c>
-      <c r="D18" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1">
-        <v>13</v>
-      </c>
-      <c r="C19" s="1">
-        <v>4.8800000000000003E-2</v>
-      </c>
-      <c r="D19" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1">
-        <v>4.2599999999999999E-2</v>
-      </c>
-      <c r="D20" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>12</v>
-      </c>
-      <c r="B21" s="1">
-        <v>13</v>
-      </c>
-      <c r="C21" s="1">
-        <v>4.8800000000000003E-2</v>
-      </c>
-      <c r="D21" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>12</v>
-      </c>
-      <c r="B22" s="1">
-        <v>23</v>
-      </c>
-      <c r="C22" s="1">
-        <v>9.8500000000000004E-2</v>
-      </c>
-      <c r="D22" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>23</v>
-      </c>
-      <c r="C23" s="1">
-        <v>8.8400000000000006E-2</v>
-      </c>
-      <c r="D23" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>14</v>
-      </c>
-      <c r="B24" s="1">
-        <v>16</v>
-      </c>
-      <c r="C24" s="1">
-        <v>5.9400000000000001E-2</v>
-      </c>
-      <c r="D24" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>15</v>
-      </c>
-      <c r="B25" s="1">
-        <v>16</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1.72E-2</v>
-      </c>
-      <c r="D25" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>15</v>
-      </c>
-      <c r="B26" s="1">
-        <v>21</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2.4900000000000002E-2</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>15</v>
-      </c>
-      <c r="B27" s="1">
-        <v>24</v>
-      </c>
-      <c r="C27" s="1">
-        <v>5.2900000000000003E-2</v>
-      </c>
-      <c r="D27" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>16</v>
-      </c>
-      <c r="B28" s="1">
-        <v>17</v>
-      </c>
-      <c r="C28" s="1">
-        <v>2.63E-2</v>
-      </c>
-      <c r="D28" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>16</v>
-      </c>
-      <c r="B29" s="1">
-        <v>19</v>
-      </c>
-      <c r="C29" s="1">
-        <v>2.3400000000000001E-2</v>
-      </c>
-      <c r="D29" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>17</v>
-      </c>
-      <c r="B30" s="1">
-        <v>18</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1.43E-2</v>
-      </c>
-      <c r="D30" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>17</v>
-      </c>
-      <c r="B31" s="1">
-        <v>22</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0.10690000000000001</v>
-      </c>
-      <c r="D31" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>18</v>
-      </c>
-      <c r="B32" s="1">
-        <v>21</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1.32E-2</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>19</v>
-      </c>
-      <c r="B33" s="1">
-        <v>20</v>
-      </c>
-      <c r="C33" s="1">
-        <v>2.0300000000000002E-2</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>20</v>
-      </c>
-      <c r="B34" s="1">
-        <v>23</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1.12E-2</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>21</v>
-      </c>
-      <c r="B35" s="1">
-        <v>22</v>
-      </c>
-      <c r="C35" s="1">
-        <v>6.9199999999999998E-2</v>
-      </c>
-      <c r="D35" s="1">
-        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -2480,24 +2123,641 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D667A1-F40E-42FE-98A4-7969DB61290E}">
+  <dimension ref="A1:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.46E-2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>175</v>
+      </c>
+      <c r="E2" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.2253</v>
+      </c>
+      <c r="D3" s="1">
+        <v>175</v>
+      </c>
+      <c r="E3" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9.0700000000000003E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>350</v>
+      </c>
+      <c r="E4" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.1356</v>
+      </c>
+      <c r="D5" s="1">
+        <v>175</v>
+      </c>
+      <c r="E5" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="D6" s="1">
+        <v>175</v>
+      </c>
+      <c r="E6" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.12710000000000002</v>
+      </c>
+      <c r="D7" s="1">
+        <v>175</v>
+      </c>
+      <c r="E7" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>400</v>
+      </c>
+      <c r="E8" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.111</v>
+      </c>
+      <c r="D9" s="1">
+        <v>175</v>
+      </c>
+      <c r="E9" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9.4E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>350</v>
+      </c>
+      <c r="E10" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6.4200000000000007E-2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>175</v>
+      </c>
+      <c r="E11" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6.5200000000000008E-2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>350</v>
+      </c>
+      <c r="E12" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.1762</v>
+      </c>
+      <c r="D13" s="1">
+        <v>175</v>
+      </c>
+      <c r="E13" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.1762</v>
+      </c>
+      <c r="D14" s="1">
+        <v>175</v>
+      </c>
+      <c r="E14" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>400</v>
+      </c>
+      <c r="E15" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>400</v>
+      </c>
+      <c r="E16" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>400</v>
+      </c>
+      <c r="E17" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>400</v>
+      </c>
+      <c r="E18" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4.8800000000000003E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>500</v>
+      </c>
+      <c r="E19" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>500</v>
+      </c>
+      <c r="E20" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1">
+        <v>13</v>
+      </c>
+      <c r="C21" s="1">
+        <v>4.8800000000000003E-2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>500</v>
+      </c>
+      <c r="E21" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>500</v>
+      </c>
+      <c r="E22" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1">
+        <v>8.8400000000000006E-2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>500</v>
+      </c>
+      <c r="E23" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1">
+        <v>16</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5.9400000000000001E-2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>500</v>
+      </c>
+      <c r="E24" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>15</v>
+      </c>
+      <c r="B25" s="1">
+        <v>16</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1.72E-2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>500</v>
+      </c>
+      <c r="E25" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>15</v>
+      </c>
+      <c r="B26" s="1">
+        <v>21</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2.4900000000000002E-2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E26" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>15</v>
+      </c>
+      <c r="B27" s="1">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5.2900000000000003E-2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>500</v>
+      </c>
+      <c r="E27" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1">
+        <v>17</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2.63E-2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>500</v>
+      </c>
+      <c r="E28" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1">
+        <v>19</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2.3400000000000001E-2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>500</v>
+      </c>
+      <c r="E29" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>17</v>
+      </c>
+      <c r="B30" s="1">
+        <v>18</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1.43E-2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>500</v>
+      </c>
+      <c r="E30" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>17</v>
+      </c>
+      <c r="B31" s="1">
+        <v>22</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.10690000000000001</v>
+      </c>
+      <c r="D31" s="1">
+        <v>500</v>
+      </c>
+      <c r="E31" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>18</v>
+      </c>
+      <c r="B32" s="1">
+        <v>21</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1.32E-2</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>19</v>
+      </c>
+      <c r="B33" s="1">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2.0300000000000002E-2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>20</v>
+      </c>
+      <c r="B34" s="1">
+        <v>23</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1.12E-2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>21</v>
+      </c>
+      <c r="B35" s="1">
+        <v>22</v>
+      </c>
+      <c r="C35" s="1">
+        <v>6.9199999999999998E-2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>500</v>
+      </c>
+      <c r="E35" s="1">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63BB4DA-7026-4DB7-9B24-BE42F9A5634C}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2588,7 +2848,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>0.60000000000000009</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2697,11 +2957,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDB7F6A-CE82-4E52-B255-E07EA147DBBD}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -2709,10 +2969,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2720,7 +2980,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2728,7 +2988,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2736,15 +2996,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2752,7 +3012,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2760,7 +3020,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2768,7 +3028,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2776,79 +3036,79 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data loading in Network
</commit_message>
<xml_diff>
--- a/Assignment 1/data.xlsx
+++ b/Assignment 1/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frede\Documents\DTU\2024\Renewables in Electricity Markets\renew-in-elec-markets\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC391156-33BA-418F-9434-728A03CAC72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD883C61-412A-419E-AFE2-7E88E594961E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gen_technical" sheetId="1" r:id="rId1"/>
@@ -1252,7 +1252,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B1" sqref="B1:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2744,7 +2744,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added more data loading
</commit_message>
<xml_diff>
--- a/Assignment 1/data.xlsx
+++ b/Assignment 1/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwitt\OneDrive\Dokumenter\GitHub\renew-in-elec-markets\Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frede\Documents\DTU\2024\Renewables in Electricity Markets\renew-in-elec-markets\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04E80B24-7FA8-46E3-AAE0-2EF644EBDC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250253B8-FCE8-4EFB-AFA1-434ED3B09DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2750,7 +2750,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>